<commit_message>
The latest version of program with FilesHelper and Converter.
</commit_message>
<xml_diff>
--- a/example_excel_histogram.xlsx
+++ b/example_excel_histogram.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewenraf\Documents\studia\Semestr VI\Projekt grupowy\synchronizowany_github\Projekt_grupowy_mion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05E435D0-D1E0-46FB-A061-AA639B165BA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D0AD02-F44F-4F13-91CA-6F73B6004B49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="histogram_six60MHz" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,13 +632,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -646,11 +652,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Procentowa</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" baseline="0"/>
-              <a:t> częstość tłumienia</a:t>
+              <a:t>Procentowa częstość tłumienia</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -668,13 +670,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -695,15 +703,100 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>histogram_six60MHz!$A$1:$A$10</c:f>
@@ -788,15 +881,16 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="490803560"/>
         <c:axId val="441140744"/>
       </c:barChart>
@@ -813,11 +907,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -831,9 +925,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -862,9 +955,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -890,9 +983,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -927,17 +1019,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -980,13 +1083,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -1012,13 +1121,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -1039,13 +1154,42 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -1139,8 +1283,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="642394632"/>
         <c:axId val="642395288"/>
       </c:barChart>
@@ -1157,11 +1301,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1175,9 +1319,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1206,9 +1349,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1234,9 +1377,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1271,17 +1413,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1384,35 +1537,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1420,26 +1571,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1448,9 +1607,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1469,14 +1627,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1485,35 +1635,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1525,30 +1675,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1564,21 +1715,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1588,20 +1736,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1612,17 +1760,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1631,14 +1779,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1650,28 +1797,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1683,17 +1824,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1702,17 +1842,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1721,17 +1861,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1740,27 +1879,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1768,11 +1906,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1780,14 +1928,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1799,12 +1947,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1813,14 +1968,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1829,9 +1983,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1841,7 +1994,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1849,9 +2002,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1862,9 +2015,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1874,48 +2026,40 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1923,26 +2067,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1951,9 +2103,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1972,14 +2123,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1988,35 +2131,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2028,30 +2171,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2067,21 +2211,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2091,20 +2232,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2115,17 +2256,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2134,14 +2275,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2153,28 +2293,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2186,17 +2320,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2205,17 +2338,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2224,17 +2357,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2243,27 +2375,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2271,11 +2402,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2283,14 +2424,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2302,12 +2443,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2316,14 +2464,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2332,9 +2479,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2344,7 +2490,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2352,9 +2498,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2365,9 +2511,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2377,14 +2522,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2762,10 +2901,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Y59" sqref="Y59"/>
     </sheetView>
   </sheetViews>

</xml_diff>